<commit_message>
Ajustes finales y resultados de otros experimentos
Se realizaron correcciones menores al código y se automatizó el uso de las listas negra y blanca para el aprendizaje de estructura de la funcion HC de bnlearn en R.

Se incluyen los resultados de nuevos experimentos ejecutados.
</commit_message>
<xml_diff>
--- a/ExperimentosR/Analisis Métricas.xlsx
+++ b/ExperimentosR/Analisis Métricas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/019bcfd77d9770ed/Documentos/MAGISTER/SEMINARIO II/Programa BN/tesis2BN/ExperimentosR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{88BB5612-E616-4069-97EE-01D9AB8DB8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{506887E8-D8F9-476C-BCE6-ED6EE468BF13}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{88BB5612-E616-4069-97EE-01D9AB8DB8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{773C027D-2CEC-4DE5-AC9C-67F6FF3149CF}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-252" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{D18EDC41-0F32-4E4C-833E-D13DFBCAE797}"/>
   </bookViews>
@@ -162,24 +162,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -189,7 +182,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -222,7 +215,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -234,24 +227,26 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18529,11 +18524,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3646585-E4C8-4489-80D5-63489859B4B3}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18551,621 +18545,615 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="11" t="s">
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="7" t="s">
+    <row r="2" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="8">
+      <c r="D2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="21">
         <v>0.84994280485014806</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="21">
         <v>0.64480362487048593</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="21">
         <v>0.10491878288721102</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="21">
         <v>0.83815136000200174</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="21">
         <v>0.84994280485014806</v>
       </c>
-      <c r="J2" s="12">
+      <c r="J2" s="10">
         <v>0.66415758271179937</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="7" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="8">
+      <c r="D3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12">
         <v>0.84998856097002895</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="12">
         <v>0.60186498412039691</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="12">
         <v>0.10491878288721102</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="12">
         <v>0.85937165795580894</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="12">
         <v>0.84998856097002895</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="12">
         <v>0.59261331038439435</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="7" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
+      <c r="D4" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12">
         <v>0.86511095859071074</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="12">
         <v>0.62988633515888526</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="12">
         <v>0.10491878288721102</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="12">
         <v>0.8797350456832721</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="12">
         <v>0.86511095859071074</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="12">
         <v>0.60100401606425646</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="16" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="15">
+      <c r="D5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="16">
         <v>0.88865248226950266</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="16">
         <v>0.69350102259118374</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="16">
         <v>0.10491878288721102</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="16">
         <v>0.93039588231672943</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="16">
         <v>0.88865248226950266</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="16">
         <v>0.59542646777586494</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="7" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="8">
+      <c r="D6" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12">
         <v>0.4900709219858152</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="12">
         <v>0.55328188957091684</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="12">
         <v>0.10491878288721102</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="12">
         <v>0.69848138531400006</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="12">
         <v>0.4900709219858152</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="12">
         <v>0.61715911264103984</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="18" t="s">
+      <c r="A7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8">
+      <c r="D7" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="12">
         <v>0.70663463738274945</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="12">
         <v>0.55206839688916587</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="12">
         <v>0.10491878288721102</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="12">
         <v>0.66865335993996078</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="12">
         <v>0.70663463738274945</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="13">
         <v>0.60179957926945826</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="A8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="8">
+      <c r="D8" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12">
         <v>0.71292610386639155</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="12">
         <v>0.54919465345627594</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="12">
         <v>0.10491878288721102</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="12">
         <v>0.67138067122888978</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="12">
         <v>0.71292610386639155</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="12">
         <v>0.58985943775100358</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="18" t="s">
+    <row r="9" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="8">
+      <c r="D9" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="18">
         <v>0.88652482269503463</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="18">
         <v>0.68947785347010127</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="18">
         <v>0.10491878288721102</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="18">
         <v>0.90444573163611286</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="18">
         <v>0.88652482269503463</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="18">
         <v>0.64927232740485741</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="A10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8">
+      <c r="D10" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="12">
         <v>0.78590711507664079</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="12">
         <v>0.53853170780572079</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="12">
         <v>0.10491878288721102</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="12">
         <v>0.75132001877497179</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="12">
         <v>0.78590711507664079</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="12">
         <v>0.55678427997705049</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="7" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="8">
+      <c r="D11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="12">
         <v>0.92666198334074035</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="12">
         <v>0.83988766014491012</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="12">
         <v>0.10492466057834279</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="12">
         <v>0.94711599679137071</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="12">
         <v>0.92666198334074035</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="12">
         <v>0.72254705858088586</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="7" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="8">
+      <c r="D12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="12">
         <v>0.91648865249243683</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="12">
         <v>0.91186197682099268</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="12">
         <v>0.10492466057834279</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="13">
         <v>0.97015675445768323</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="12">
         <v>0.91648865249243683</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="12">
         <v>0.63150312463477154</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="7" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="8">
+      <c r="D13" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="12">
         <v>0.89884015999770561</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="12">
         <v>0.74537353922513705</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="12">
         <v>0.10492466057834279</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="12">
         <v>0.90961985709451609</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="12">
         <v>0.89884015999770561</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="12">
         <v>0.68643128209711413</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="7" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="8">
+      <c r="D14" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="12">
         <v>0.91702484552192742</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="12">
         <v>0.92299642076365573</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="12">
         <v>0.10492466057834279</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="9">
         <v>0.97116731325347572</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="12">
         <v>0.91702484552192742</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="12">
         <v>0.63180252583237628</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="7" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="8">
+      <c r="D15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="12">
         <v>0.70087740677552979</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="12">
         <v>0.74486664301937044</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="12">
         <v>0.10492466057834279</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="12">
         <v>0.86948653422639011</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="12">
         <v>0.70087740677552979</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="12">
         <v>0.81716027187874496</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="18" t="s">
+      <c r="A16" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="8">
+      <c r="D16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="12">
         <v>0.86512110108141871</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="12">
         <v>0.87793492624530756</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="12">
         <v>0.5</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="12">
         <v>0.883048681986215</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="12">
         <v>0.86512110108141871</v>
       </c>
-      <c r="J16" s="20">
+      <c r="J16" s="12">
         <v>0.86512110108141882</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="A17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="8">
+      <c r="D17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="12">
         <v>0.84152560550540656</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="12">
         <v>0.84423481740997397</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="12">
         <v>0.5</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="12">
         <v>0.84541901809117037</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="12">
         <v>0.84152560550540656</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="12">
         <v>0.84152560550540656</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="18" t="s">
+      <c r="A18" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="14">
+      <c r="D18" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="13">
         <v>0.95305836089015938</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="13">
         <v>0.95344412966292147</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="12">
         <v>0.5</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="12">
         <v>0.95347463615207961</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="13">
         <v>0.95305836089015938</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="13">
         <v>0.95305836089015938</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="A19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="8">
+      <c r="D19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="12">
         <v>0.84419697917597603</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="12">
         <v>0.8453257832234311</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="12">
         <v>0.5</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="12">
         <v>0.84585159449010983</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="12">
         <v>0.84419697917597603</v>
       </c>
-      <c r="J19" s="8">
+      <c r="J19" s="12">
         <v>0.84419697917597603</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J19" xr:uid="{E3646585-E4C8-4489-80D5-63489859B4B3}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="SI"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J19" xr:uid="{E3646585-E4C8-4489-80D5-63489859B4B3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>